<commit_message>
S-01242 Add processor function to intabulate dyad sequences. Functional
</commit_message>
<xml_diff>
--- a/catsmat/Documentation/Trigram results for Proportional canons.xlsx
+++ b/catsmat/Documentation/Trigram results for Proportional canons.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="235" uniqueCount="229">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="267" uniqueCount="255">
   <si>
     <t>trigrams</t>
   </si>
@@ -706,6 +706,84 @@
   </si>
   <si>
     <t xml:space="preserve">undefined </t>
+  </si>
+  <si>
+    <t>contour duples</t>
+  </si>
+  <si>
+    <t>leapdown-leapdown</t>
+  </si>
+  <si>
+    <t>leapdown-stepdown</t>
+  </si>
+  <si>
+    <t>leapdown-repeat</t>
+  </si>
+  <si>
+    <t>leapdown-stepup</t>
+  </si>
+  <si>
+    <t>leapdown-leapup</t>
+  </si>
+  <si>
+    <t xml:space="preserve">leapdown-undefined </t>
+  </si>
+  <si>
+    <t>stepdown-leapdown</t>
+  </si>
+  <si>
+    <t>stepdown-repeat</t>
+  </si>
+  <si>
+    <t>stepdown-stepup</t>
+  </si>
+  <si>
+    <t>stepdown-leapup</t>
+  </si>
+  <si>
+    <t>repeat-leapdown</t>
+  </si>
+  <si>
+    <t>repeat-stepdown</t>
+  </si>
+  <si>
+    <t>repeat-repeat</t>
+  </si>
+  <si>
+    <t>repeat-stepup</t>
+  </si>
+  <si>
+    <t>repeat-leapup</t>
+  </si>
+  <si>
+    <t xml:space="preserve">repeat-undefined </t>
+  </si>
+  <si>
+    <t>stepup-leapdown</t>
+  </si>
+  <si>
+    <t>stepup-stepdown</t>
+  </si>
+  <si>
+    <t>stepup-repeat</t>
+  </si>
+  <si>
+    <t>stepup-leapup</t>
+  </si>
+  <si>
+    <t>leapup-leapdown</t>
+  </si>
+  <si>
+    <t>leapup-stepdown</t>
+  </si>
+  <si>
+    <t>leapup-repeat</t>
+  </si>
+  <si>
+    <t>leapup-stepup</t>
+  </si>
+  <si>
+    <t>leapup-leapup</t>
   </si>
 </sst>
 </file>
@@ -1075,10 +1153,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:HG20"/>
+  <dimension ref="A1:HG30"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A19" sqref="A19:XFD20"/>
+    <sheetView tabSelected="1" topLeftCell="M6" workbookViewId="0">
+      <selection activeCell="AB30" sqref="AB30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -5692,7 +5770,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="17" spans="1:7">
+    <row r="17" spans="1:28">
       <c r="A17" t="s">
         <v>217</v>
       </c>
@@ -5715,7 +5793,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="18" spans="1:7">
+    <row r="18" spans="1:28">
       <c r="A18" t="s">
         <v>218</v>
       </c>
@@ -5738,7 +5816,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="19" spans="1:7">
+    <row r="19" spans="1:28">
       <c r="A19" t="s">
         <v>219</v>
       </c>
@@ -5761,7 +5839,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="20" spans="1:7">
+    <row r="20" spans="1:28">
       <c r="A20" t="s">
         <v>220</v>
       </c>
@@ -5784,9 +5862,597 @@
         <v>7</v>
       </c>
     </row>
+    <row r="24" spans="1:28">
+      <c r="A24" t="s">
+        <v>229</v>
+      </c>
+      <c r="B24" t="s">
+        <v>230</v>
+      </c>
+      <c r="C24" t="s">
+        <v>234</v>
+      </c>
+      <c r="D24" t="s">
+        <v>250</v>
+      </c>
+      <c r="E24" t="s">
+        <v>254</v>
+      </c>
+      <c r="F24" t="s">
+        <v>236</v>
+      </c>
+      <c r="G24" t="s">
+        <v>231</v>
+      </c>
+      <c r="H24" t="s">
+        <v>253</v>
+      </c>
+      <c r="I24" t="s">
+        <v>240</v>
+      </c>
+      <c r="J24" t="s">
+        <v>249</v>
+      </c>
+      <c r="K24" t="s">
+        <v>232</v>
+      </c>
+      <c r="L24" t="s">
+        <v>244</v>
+      </c>
+      <c r="M24" t="s">
+        <v>252</v>
+      </c>
+      <c r="N24" t="s">
+        <v>242</v>
+      </c>
+      <c r="O24" t="s">
+        <v>247</v>
+      </c>
+      <c r="P24" t="s">
+        <v>238</v>
+      </c>
+      <c r="Q24" t="s">
+        <v>251</v>
+      </c>
+      <c r="R24" t="s">
+        <v>239</v>
+      </c>
+      <c r="S24" t="s">
+        <v>246</v>
+      </c>
+      <c r="T24" t="s">
+        <v>233</v>
+      </c>
+      <c r="U24" t="s">
+        <v>241</v>
+      </c>
+      <c r="V24" t="s">
+        <v>237</v>
+      </c>
+      <c r="W24" t="s">
+        <v>248</v>
+      </c>
+      <c r="X24" t="s">
+        <v>243</v>
+      </c>
+      <c r="Y24" t="s">
+        <v>235</v>
+      </c>
+      <c r="Z24" t="s">
+        <v>245</v>
+      </c>
+    </row>
+    <row r="25" spans="1:28">
+      <c r="A25" t="s">
+        <v>215</v>
+      </c>
+      <c r="B25">
+        <v>30</v>
+      </c>
+      <c r="C25">
+        <v>24</v>
+      </c>
+      <c r="D25">
+        <v>22</v>
+      </c>
+      <c r="E25">
+        <v>21</v>
+      </c>
+      <c r="F25">
+        <v>10</v>
+      </c>
+      <c r="G25">
+        <v>11</v>
+      </c>
+      <c r="H25">
+        <v>10</v>
+      </c>
+      <c r="I25">
+        <v>6</v>
+      </c>
+      <c r="J25">
+        <v>8</v>
+      </c>
+      <c r="K25">
+        <v>4</v>
+      </c>
+      <c r="L25">
+        <v>7</v>
+      </c>
+      <c r="M25">
+        <v>10</v>
+      </c>
+      <c r="N25">
+        <v>3</v>
+      </c>
+      <c r="O25">
+        <v>7</v>
+      </c>
+      <c r="P25">
+        <v>5</v>
+      </c>
+      <c r="Q25">
+        <v>0</v>
+      </c>
+      <c r="R25">
+        <v>3</v>
+      </c>
+      <c r="S25">
+        <v>4</v>
+      </c>
+      <c r="T25">
+        <v>3</v>
+      </c>
+      <c r="U25">
+        <v>0</v>
+      </c>
+      <c r="V25">
+        <v>2</v>
+      </c>
+      <c r="W25">
+        <v>0</v>
+      </c>
+      <c r="X25">
+        <v>1</v>
+      </c>
+      <c r="Y25">
+        <v>0</v>
+      </c>
+      <c r="Z25">
+        <v>1</v>
+      </c>
+      <c r="AA25">
+        <f>SUM(B25:Z25)</f>
+        <v>192</v>
+      </c>
+    </row>
+    <row r="26" spans="1:28">
+      <c r="A26" t="s">
+        <v>216</v>
+      </c>
+      <c r="B26">
+        <v>25</v>
+      </c>
+      <c r="C26">
+        <v>27</v>
+      </c>
+      <c r="D26">
+        <v>28</v>
+      </c>
+      <c r="E26">
+        <v>20</v>
+      </c>
+      <c r="F26">
+        <v>3</v>
+      </c>
+      <c r="G26">
+        <v>4</v>
+      </c>
+      <c r="H26">
+        <v>4</v>
+      </c>
+      <c r="I26">
+        <v>7</v>
+      </c>
+      <c r="J26">
+        <v>5</v>
+      </c>
+      <c r="K26">
+        <v>12</v>
+      </c>
+      <c r="L26">
+        <v>14</v>
+      </c>
+      <c r="M26">
+        <v>10</v>
+      </c>
+      <c r="N26">
+        <v>8</v>
+      </c>
+      <c r="O26">
+        <v>2</v>
+      </c>
+      <c r="P26">
+        <v>0</v>
+      </c>
+      <c r="Q26">
+        <v>3</v>
+      </c>
+      <c r="R26">
+        <v>7</v>
+      </c>
+      <c r="S26">
+        <v>0</v>
+      </c>
+      <c r="T26">
+        <v>0</v>
+      </c>
+      <c r="U26">
+        <v>1</v>
+      </c>
+      <c r="V26">
+        <v>0</v>
+      </c>
+      <c r="W26">
+        <v>0</v>
+      </c>
+      <c r="X26">
+        <v>1</v>
+      </c>
+      <c r="Y26">
+        <v>0</v>
+      </c>
+      <c r="Z26">
+        <v>2</v>
+      </c>
+      <c r="AA26">
+        <f t="shared" ref="AA26:AA29" si="0">SUM(B26:Z26)</f>
+        <v>183</v>
+      </c>
+    </row>
+    <row r="27" spans="1:28">
+      <c r="A27" t="s">
+        <v>217</v>
+      </c>
+      <c r="B27">
+        <v>18</v>
+      </c>
+      <c r="C27">
+        <v>16</v>
+      </c>
+      <c r="D27">
+        <v>10</v>
+      </c>
+      <c r="E27">
+        <v>9</v>
+      </c>
+      <c r="F27">
+        <v>13</v>
+      </c>
+      <c r="G27">
+        <v>8</v>
+      </c>
+      <c r="H27">
+        <v>10</v>
+      </c>
+      <c r="I27">
+        <v>3</v>
+      </c>
+      <c r="J27">
+        <v>4</v>
+      </c>
+      <c r="K27">
+        <v>4</v>
+      </c>
+      <c r="L27">
+        <v>1</v>
+      </c>
+      <c r="M27">
+        <v>0</v>
+      </c>
+      <c r="N27">
+        <v>2</v>
+      </c>
+      <c r="O27">
+        <v>3</v>
+      </c>
+      <c r="P27">
+        <v>1</v>
+      </c>
+      <c r="Q27">
+        <v>0</v>
+      </c>
+      <c r="R27">
+        <v>0</v>
+      </c>
+      <c r="S27">
+        <v>3</v>
+      </c>
+      <c r="T27">
+        <v>1</v>
+      </c>
+      <c r="U27">
+        <v>2</v>
+      </c>
+      <c r="V27">
+        <v>0</v>
+      </c>
+      <c r="W27">
+        <v>0</v>
+      </c>
+      <c r="X27">
+        <v>0</v>
+      </c>
+      <c r="Y27">
+        <v>0</v>
+      </c>
+      <c r="Z27">
+        <v>0</v>
+      </c>
+      <c r="AA27">
+        <f t="shared" si="0"/>
+        <v>108</v>
+      </c>
+    </row>
+    <row r="28" spans="1:28">
+      <c r="A28" t="s">
+        <v>218</v>
+      </c>
+      <c r="B28">
+        <v>96</v>
+      </c>
+      <c r="C28">
+        <v>93</v>
+      </c>
+      <c r="D28">
+        <v>80</v>
+      </c>
+      <c r="E28">
+        <v>35</v>
+      </c>
+      <c r="F28">
+        <v>53</v>
+      </c>
+      <c r="G28">
+        <v>47</v>
+      </c>
+      <c r="H28">
+        <v>36</v>
+      </c>
+      <c r="I28">
+        <v>39</v>
+      </c>
+      <c r="J28">
+        <v>25</v>
+      </c>
+      <c r="K28">
+        <v>20</v>
+      </c>
+      <c r="L28">
+        <v>13</v>
+      </c>
+      <c r="M28">
+        <v>12</v>
+      </c>
+      <c r="N28">
+        <v>14</v>
+      </c>
+      <c r="O28">
+        <v>12</v>
+      </c>
+      <c r="P28">
+        <v>7</v>
+      </c>
+      <c r="Q28">
+        <v>17</v>
+      </c>
+      <c r="R28">
+        <v>8</v>
+      </c>
+      <c r="S28">
+        <v>11</v>
+      </c>
+      <c r="T28">
+        <v>9</v>
+      </c>
+      <c r="U28">
+        <v>6</v>
+      </c>
+      <c r="V28">
+        <v>6</v>
+      </c>
+      <c r="W28">
+        <v>6</v>
+      </c>
+      <c r="X28">
+        <v>3</v>
+      </c>
+      <c r="Y28">
+        <v>4</v>
+      </c>
+      <c r="Z28">
+        <v>0</v>
+      </c>
+      <c r="AA28">
+        <f t="shared" si="0"/>
+        <v>652</v>
+      </c>
+    </row>
+    <row r="29" spans="1:28">
+      <c r="A29" t="s">
+        <v>219</v>
+      </c>
+      <c r="B29">
+        <v>16</v>
+      </c>
+      <c r="C29">
+        <v>13</v>
+      </c>
+      <c r="D29">
+        <v>13</v>
+      </c>
+      <c r="E29">
+        <v>3</v>
+      </c>
+      <c r="F29">
+        <v>6</v>
+      </c>
+      <c r="G29">
+        <v>10</v>
+      </c>
+      <c r="H29">
+        <v>5</v>
+      </c>
+      <c r="I29">
+        <v>6</v>
+      </c>
+      <c r="J29">
+        <v>4</v>
+      </c>
+      <c r="K29">
+        <v>2</v>
+      </c>
+      <c r="L29">
+        <v>6</v>
+      </c>
+      <c r="M29">
+        <v>4</v>
+      </c>
+      <c r="N29">
+        <v>4</v>
+      </c>
+      <c r="O29">
+        <v>2</v>
+      </c>
+      <c r="P29">
+        <v>7</v>
+      </c>
+      <c r="Q29">
+        <v>0</v>
+      </c>
+      <c r="R29">
+        <v>0</v>
+      </c>
+      <c r="S29">
+        <v>0</v>
+      </c>
+      <c r="T29">
+        <v>0</v>
+      </c>
+      <c r="U29">
+        <v>2</v>
+      </c>
+      <c r="V29">
+        <v>1</v>
+      </c>
+      <c r="W29">
+        <v>1</v>
+      </c>
+      <c r="X29">
+        <v>0</v>
+      </c>
+      <c r="Y29">
+        <v>0</v>
+      </c>
+      <c r="Z29">
+        <v>0</v>
+      </c>
+      <c r="AA29">
+        <f t="shared" si="0"/>
+        <v>105</v>
+      </c>
+      <c r="AB29">
+        <f>SUM(AA25:AA29)</f>
+        <v>1240</v>
+      </c>
+    </row>
+    <row r="30" spans="1:28">
+      <c r="A30" t="s">
+        <v>220</v>
+      </c>
+      <c r="B30">
+        <v>185</v>
+      </c>
+      <c r="C30">
+        <v>173</v>
+      </c>
+      <c r="D30">
+        <v>153</v>
+      </c>
+      <c r="E30">
+        <v>88</v>
+      </c>
+      <c r="F30">
+        <v>85</v>
+      </c>
+      <c r="G30">
+        <v>80</v>
+      </c>
+      <c r="H30">
+        <v>65</v>
+      </c>
+      <c r="I30">
+        <v>61</v>
+      </c>
+      <c r="J30">
+        <v>46</v>
+      </c>
+      <c r="K30">
+        <v>42</v>
+      </c>
+      <c r="L30">
+        <v>41</v>
+      </c>
+      <c r="M30">
+        <v>36</v>
+      </c>
+      <c r="N30">
+        <v>31</v>
+      </c>
+      <c r="O30">
+        <v>26</v>
+      </c>
+      <c r="P30">
+        <v>20</v>
+      </c>
+      <c r="Q30">
+        <v>20</v>
+      </c>
+      <c r="R30">
+        <v>18</v>
+      </c>
+      <c r="S30">
+        <v>18</v>
+      </c>
+      <c r="T30">
+        <v>13</v>
+      </c>
+      <c r="U30">
+        <v>11</v>
+      </c>
+      <c r="V30">
+        <v>9</v>
+      </c>
+      <c r="W30">
+        <v>7</v>
+      </c>
+      <c r="X30">
+        <v>5</v>
+      </c>
+      <c r="Y30">
+        <v>4</v>
+      </c>
+      <c r="Z30">
+        <v>3</v>
+      </c>
+      <c r="AA30">
+        <f>SUM(B30:Z30)</f>
+        <v>1240</v>
+      </c>
+    </row>
   </sheetData>
-  <sortState columnSort="1" ref="A2:HG8">
-    <sortCondition descending="1" ref="A8:HG8"/>
+  <sortState columnSort="1" ref="A24:Z30">
+    <sortCondition descending="1" ref="A30:Z30"/>
   </sortState>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <extLst>

</xml_diff>